<commit_message>
Contacts & Reports changes latest - 30 Mar 2023
</commit_message>
<xml_diff>
--- a/TestData/T2244_Contacts_DuplicateManagement_Edit_Contact_Record_ToMatchWithAnExistingContact.xlsx
+++ b/TestData/T2244_Contacts_DuplicateManagement_Edit_Contact_Record_ToMatchWithAnExistingContact.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HL\SalesForce_Project\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF47A6F2-D762-4ECD-A361-1B12331E8AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBD4F2C-BB09-48C1-8F77-1A435C0057FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,13 +105,13 @@
     <t>Kansas</t>
   </si>
   <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
     <t>Test Test</t>
   </si>
   <si>
     <t>(522) 555-5555</t>
+  </si>
+  <si>
+    <t>testtest@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,13 +546,13 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>

</xml_diff>